<commit_message>
acp test is happening
</commit_message>
<xml_diff>
--- a/CSV/i2c_test_newMotor_calc.xlsx
+++ b/CSV/i2c_test_newMotor_calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ditte\aauRepo\esd7_git\3Dprinter-BLDC-control\CSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AFD5D1-97FE-4E5B-B7B4-C1F9820B0723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72A3645-5422-45BD-BA32-A13F885E6610}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{2F789D5C-9A6C-4541-9F57-B1D731EE9AE8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{2F789D5C-9A6C-4541-9F57-B1D731EE9AE8}"/>
   </bookViews>
   <sheets>
     <sheet name="i2c_test_newMotor" sheetId="1" r:id="rId1"/>
@@ -11403,12 +11403,20 @@
             </a:r>
             <a:r>
               <a:rPr lang="da-DK" baseline="0"/>
-              <a:t> of speed/placement for the two motors</a:t>
+              <a:t> speed, taken at percentage of rotation, for the two motors</a:t>
             </a:r>
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18295905084181111"/>
+          <c:y val="2.3036275422434502E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12178,7 +12186,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="da-DK"/>
-                  <a:t>Rotation placement</a:t>
+                  <a:t>Percentage of roatation</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -24859,8 +24867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7199684-7DFC-4EDE-86A9-23A6551E4DBC}">
   <dimension ref="A1:AE1172"/>
   <sheetViews>
-    <sheetView topLeftCell="U81" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="AF88" sqref="AF88"/>
+    <sheetView tabSelected="1" topLeftCell="T79" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Y88" sqref="Y88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -47092,7 +47100,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DDFF37-94BC-43BE-9F50-59DEE3D64DFD}">
   <dimension ref="A1:E836"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E120" sqref="D2:E120"/>
     </sheetView>
   </sheetViews>
@@ -49261,7 +49269,7 @@
         <v>1</v>
       </c>
       <c r="D121" t="e">
-        <f t="shared" ref="D69:D130" si="2">(C121-C120)/1000000 +D120</f>
+        <f t="shared" ref="D121:D130" si="2">(C121-C120)/1000000 +D120</f>
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>